<commit_message>
Modelos actualizados con función validacion
</commit_message>
<xml_diff>
--- a/results_cv.xlsx
+++ b/results_cv.xlsx
@@ -463,23 +463,23 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>RANDOM FOREST VGG16 PCA</t>
+          <t>Regresión Logística gray</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5247282509323995</v>
+        <v>0.2377205781933585</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5106406958904053</v>
+        <v>0.2369306836345303</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5105595000016662</v>
+        <v>0.2344130759382817</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5211864406779662</v>
+        <v>0.2454802259887006</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8107799163942339</v>
+        <v>0.5362792635039743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios para cm y roc auc
</commit_message>
<xml_diff>
--- a/results_cv.xlsx
+++ b/results_cv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -834,6 +834,50 @@
         <v>0.728394408426335</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Árbol de Decisión VGG16</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.4749160797946737</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.4727382729540192</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.471018402810777</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4782485875706216</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.7072209126229811</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Árbol de Decisión VGG16 PCA</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.5251508181845809</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.5239877280651721</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.5238354656277789</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.5338983050847459</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.6971586288526027</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>